<commit_message>
road map - edited
</commit_message>
<xml_diff>
--- a/documentation/road_map.xlsx
+++ b/documentation/road_map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sramk\Documents\vysoka_skola\bakalarka\gitKraken_bp\PluginIntoIntelliJ_BP\PluginIntoIntelliJ_BP\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053E5331-FEBD-4CE4-BF40-6A2807D2BEA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C902DC1-EC70-4C5C-89E3-E8EDE985FD1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:O12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,38 +492,36 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
@@ -534,8 +532,6 @@
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
@@ -565,8 +561,6 @@
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -596,8 +590,6 @@
       <c r="A16" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -608,8 +600,6 @@
       <c r="A17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
@@ -620,8 +610,6 @@
       <c r="A18" t="s">
         <v>14</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -632,7 +620,7 @@
       <c r="A19" t="s">
         <v>15</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">

</xml_diff>